<commit_message>
Novas planilhas e estudos
</commit_message>
<xml_diff>
--- a/Planilha Cartão de Crédito/Cartão_de_Credito.xlsx
+++ b/Planilha Cartão de Crédito/Cartão_de_Credito.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Excel Estudos\Planilha Cartão de Crédito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8210266-A2F4-402E-A28C-188FE0232628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510B79B4-F95D-46CD-980C-9D8BB854AF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A65D1B47-B366-4730-B1BA-7EC03AAC71B1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
   <si>
     <t>Janeiro</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>Kibeleza</t>
+  </si>
+  <si>
+    <t>Em Aberto</t>
   </si>
 </sst>
 </file>
@@ -380,12 +383,7 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -425,18 +423,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -802,6 +788,38 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF7030A0"/>
@@ -810,8 +828,8 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Estilo de Tabela 1" pivot="0" count="2" xr9:uid="{8A5B426F-D23F-4C28-AA1C-25955EDA2E3C}">
-      <tableStyleElement type="wholeTable" dxfId="44"/>
+    <tableStyle name="Estilo de Tabela 1" pivot="0" count="1" xr9:uid="{8A5B426F-D23F-4C28-AA1C-25955EDA2E3C}">
+      <tableStyleElement type="wholeTable" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -846,8 +864,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.6096096096096092E-3"/>
-          <c:y val="0.1102757762719999"/>
+          <c:x val="6.3698632556529345E-4"/>
+          <c:y val="0.13012032602107429"/>
           <c:w val="0.94714714714714709"/>
           <c:h val="0.77944844745600017"/>
         </c:manualLayout>
@@ -885,9 +903,9 @@
               <a:solidFill>
                 <a:srgbClr val="7030A0"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="50800">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -895,7 +913,9 @@
           </c:marker>
           <c:dLbls>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -1690,15 +1710,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>514351</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>1247774</xdr:colOff>
+      <xdr:colOff>809625</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>342900</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1713,8 +1733,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9305925" y="0"/>
-          <a:ext cx="6134099" cy="1295400"/>
+          <a:off x="9620251" y="47625"/>
+          <a:ext cx="5724524" cy="1238250"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1776,15 +1796,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1104901</xdr:colOff>
+      <xdr:colOff>962026</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1799,8 +1819,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4133851" y="47625"/>
-          <a:ext cx="3829050" cy="942975"/>
+          <a:off x="4410076" y="47625"/>
+          <a:ext cx="4010025" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1865,10 +1885,10 @@
       <xdr:rowOff>129269</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>71501</xdr:rowOff>
+      <xdr:rowOff>61976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2007,15 +2027,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
+      <xdr:colOff>238124</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2030,8 +2050,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5276849" y="533401"/>
-          <a:ext cx="1981201" cy="266700"/>
+          <a:off x="5905499" y="419101"/>
+          <a:ext cx="1981201" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2074,166 +2094,6 @@
               </a:solidFill>
             </a:rPr>
             <a:t> de Fechamento:  02 </a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1100" b="1" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Retângulo: Cantos Arredondados 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71783C31-426F-48AA-837F-FF1CC8738FB0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="219075" y="38101"/>
-          <a:ext cx="1952625" cy="361950"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="7030A0"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="44450" dist="27940" dir="5400000" algn="ctr">
-            <a:srgbClr val="000000">
-              <a:alpha val="32000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront">
-            <a:rot lat="0" lon="0" rev="0"/>
-          </a:camera>
-          <a:lightRig rig="balanced" dir="t">
-            <a:rot lat="0" lon="0" rev="8700000"/>
-          </a:lightRig>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="190500" h="38100"/>
-        </a:sp3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="CaixaDeTexto 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944244AB-306C-42F9-BEE0-1E205546E9D4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="219074" y="38100"/>
-          <a:ext cx="2028826" cy="323851"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Limite no cartão: 119,06</a:t>
           </a:r>
           <a:endParaRPr lang="pt-BR" sz="1100" b="1" baseline="0">
             <a:solidFill>
@@ -3793,15 +3653,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>628649</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="$A$67">
       <xdr:nvSpPr>
@@ -3816,7 +3676,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1019174" y="581024"/>
+          <a:off x="1000124" y="400049"/>
           <a:ext cx="1266825" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3871,15 +3731,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3894,8 +3754,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66675" y="571501"/>
-          <a:ext cx="752475" cy="390525"/>
+          <a:off x="95250" y="381001"/>
+          <a:ext cx="838200" cy="361949"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4438,6 +4298,7 @@
               <a:latin typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
+            <a:pPr/>
             <a:t> R$ 650,90 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
@@ -4550,15 +4411,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>647699</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4573,7 +4434,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9439276"/>
+          <a:off x="38100" y="9553576"/>
           <a:ext cx="1571624" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -4642,16 +4503,162 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>390525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="CaixaDeTexto 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA438282-6809-460E-9D35-06BFC38FC776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95250" y="790576"/>
+          <a:ext cx="838200" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Limite:</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1200" b="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="CaixaDeTexto 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66B1538E-9C44-4DD4-A7F2-47AC827A88B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="762001"/>
+          <a:ext cx="838200" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>R$: 90</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1200" b="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{39A8A5B2-8290-4B7F-9614-82EB65DC0B3F}" name="Tabela1" displayName="Tabela1" ref="A10:E17" totalsRowShown="0" headerRowDxfId="43" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{39A8A5B2-8290-4B7F-9614-82EB65DC0B3F}" name="Tabela1" displayName="Tabela1" ref="A10:E17" totalsRowShown="0" headerRowDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A10:E17" xr:uid="{39A8A5B2-8290-4B7F-9614-82EB65DC0B3F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8A75BB18-20EE-481B-966B-798A9EDB2CC7}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{9679229E-8637-4EAE-8972-07913B5C566A}" name="Valores" dataDxfId="41" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{4CD592F1-7EF4-405A-B4F6-BCFED22974C0}" name="Datas" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{9679229E-8637-4EAE-8972-07913B5C566A}" name="Valores" dataDxfId="38" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{4CD592F1-7EF4-405A-B4F6-BCFED22974C0}" name="Datas" dataDxfId="37"/>
     <tableColumn id="4" xr3:uid="{1788627D-ED42-4395-91ED-645536255C25}" name="Status"/>
     <tableColumn id="5" xr3:uid="{AE78BED4-698C-4613-B378-B6FA518FFC17}" name="Data de pagamento"/>
   </tableColumns>
@@ -4660,12 +4667,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9C494F9E-BBB2-48B1-9997-AA43CBD78035}" name="Tabela15910" displayName="Tabela15910" ref="G37:K43" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9C494F9E-BBB2-48B1-9997-AA43CBD78035}" name="Tabela15910" displayName="Tabela15910" ref="G37:K43" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="G37:K43" xr:uid="{9C494F9E-BBB2-48B1-9997-AA43CBD78035}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{727D733C-6756-4C6C-B6CB-CDD50C85DBDA}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{C6DFF933-D7A3-499D-97FB-CD3846C14006}" name="Valores" dataDxfId="8" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{BA5D7405-7547-4D55-B00B-A24485C31606}" name="Datas" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C6DFF933-D7A3-499D-97FB-CD3846C14006}" name="Valores" dataDxfId="5" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{BA5D7405-7547-4D55-B00B-A24485C31606}" name="Datas" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{27201F52-5800-4185-9017-7E4D5062B3C9}" name="Status"/>
     <tableColumn id="5" xr3:uid="{5DBD2B16-4113-43B8-BFC4-57B44B377773}" name="Data de pagamento"/>
   </tableColumns>
@@ -4674,12 +4681,12 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C96C312E-2166-4CCE-99C8-D0338455D50E}" name="Tabela159101117" displayName="Tabela159101117" ref="A52:E62" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{C96C312E-2166-4CCE-99C8-D0338455D50E}" name="Tabela159101117" displayName="Tabela159101117" ref="A52:E62" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A52:E62" xr:uid="{C96C312E-2166-4CCE-99C8-D0338455D50E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DBB412CB-7DE1-4BC8-9904-3EB0E65CA353}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{60242FB0-D0D1-4DF9-8C76-538240114633}" name="Valores" dataDxfId="2" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{930063A3-069E-434F-95D2-BEB123BB336C}" name="Datas" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{60242FB0-D0D1-4DF9-8C76-538240114633}" name="Valores" dataDxfId="1" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{930063A3-069E-434F-95D2-BEB123BB336C}" name="Datas" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{4860ECDF-3D3E-40D5-A0DD-0103DE04AF51}" name="Status"/>
     <tableColumn id="5" xr3:uid="{8004BAA3-9DE5-4BB6-A9F6-48974D363EA4}" name="Data de pagamento"/>
   </tableColumns>
@@ -4688,12 +4695,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6BC6B8C-EFC4-4C59-88F0-FFD31C7A7A50}" name="Tabela13" displayName="Tabela13" ref="G10:K13" totalsRowShown="0" headerRowDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6BC6B8C-EFC4-4C59-88F0-FFD31C7A7A50}" name="Tabela13" displayName="Tabela13" ref="G10:K13" totalsRowShown="0" headerRowDxfId="36" tableBorderDxfId="35">
   <autoFilter ref="G10:K13" xr:uid="{D6BC6B8C-EFC4-4C59-88F0-FFD31C7A7A50}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{6E81EDED-1185-4CCC-829F-577988709FF8}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{EDB7B9B0-F42A-44B3-AABE-1489434EB330}" name="Valores" dataDxfId="37" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{385DB38A-A100-42D4-B3A0-A9FDDE6613DE}" name="Datas" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{EDB7B9B0-F42A-44B3-AABE-1489434EB330}" name="Valores" dataDxfId="34" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{385DB38A-A100-42D4-B3A0-A9FDDE6613DE}" name="Datas" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{777D17F4-45F5-496F-B17F-5C1CC2989EDC}" name="Status"/>
     <tableColumn id="5" xr3:uid="{1B6F5ABA-0D92-4445-AC44-6A2DEC9A2D49}" name="Data de pagamento"/>
   </tableColumns>
@@ -4702,12 +4709,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC56EC66-A523-4F5C-874D-48DA4DD55D72}" name="Tabela134" displayName="Tabela134" ref="M10:Q15" totalsRowShown="0" headerRowDxfId="35" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BC56EC66-A523-4F5C-874D-48DA4DD55D72}" name="Tabela134" displayName="Tabela134" ref="M10:Q15" totalsRowShown="0" headerRowDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="M10:Q15" xr:uid="{BC56EC66-A523-4F5C-874D-48DA4DD55D72}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{412C2506-BEA7-473D-B946-89CBADA4D747}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{46A88424-B325-4843-9194-4266D9B3FBC6}" name="Valores" dataDxfId="33" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{D7D770B7-1F44-4CE4-9F6D-56BEBAA07FE6}" name="Datas" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{46A88424-B325-4843-9194-4266D9B3FBC6}" name="Valores" dataDxfId="30" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{D7D770B7-1F44-4CE4-9F6D-56BEBAA07FE6}" name="Datas" dataDxfId="29"/>
     <tableColumn id="4" xr3:uid="{DFB7664D-41C8-4FFE-850F-F027E093B58E}" name="Status"/>
     <tableColumn id="5" xr3:uid="{6366C59B-D318-42E5-8DC5-3DBF505F58DC}" name="Data de pagamento"/>
   </tableColumns>
@@ -4716,12 +4723,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C9494FA5-06D8-4345-983D-D73E7A4D6FC0}" name="Tabela15" displayName="Tabela15" ref="A22:E30" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C9494FA5-06D8-4345-983D-D73E7A4D6FC0}" name="Tabela15" displayName="Tabela15" ref="A22:E30" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
   <autoFilter ref="A22:E30" xr:uid="{C9494FA5-06D8-4345-983D-D73E7A4D6FC0}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{71FBD8AB-BC49-4881-AA3B-3376B84E4B9D}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{18C3D043-BA24-47EA-9C87-A2865934FBA1}" name="Valores" dataDxfId="29" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{5DFE398F-040B-439A-B063-5C50393FD691}" name="Datas" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{18C3D043-BA24-47EA-9C87-A2865934FBA1}" name="Valores" dataDxfId="26" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{5DFE398F-040B-439A-B063-5C50393FD691}" name="Datas" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{A7615629-FB4A-4BF2-8B30-9F0F5FECDA56}" name="Status"/>
     <tableColumn id="5" xr3:uid="{0BACD111-6BDA-4342-867A-AA0D3F25B243}" name="Data de pagamento"/>
   </tableColumns>
@@ -4734,19 +4741,19 @@
   <autoFilter ref="A69:B81" xr:uid="{405BAF61-FD21-4264-9AEA-82AF7158BF9C}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F4F218A7-E399-4E5F-BBD4-1FA7D3D7378B}" name="Meses"/>
-    <tableColumn id="2" xr3:uid="{D1D813A5-3BD5-4CC5-A904-04929AE948F2}" name="Despesas" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{D1D813A5-3BD5-4CC5-A904-04929AE948F2}" name="Despesas" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DF07F7A7-B23C-41DF-96F3-9D70FB4BCBFF}" name="Tabela157" displayName="Tabela157" ref="G22:K33" totalsRowShown="0" headerRowDxfId="26" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DF07F7A7-B23C-41DF-96F3-9D70FB4BCBFF}" name="Tabela157" displayName="Tabela157" ref="G22:K33" totalsRowShown="0" headerRowDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="G22:K33" xr:uid="{DF07F7A7-B23C-41DF-96F3-9D70FB4BCBFF}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7B72153A-1996-4BC1-855B-65DF91151DD6}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{3AF176EB-2D0F-4DAC-948F-8094D210F6B7}" name="Valores" dataDxfId="24" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{1BDBFC0F-1DB0-4CE0-9283-C7753C9A1C08}" name="Datas" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{3AF176EB-2D0F-4DAC-948F-8094D210F6B7}" name="Valores" dataDxfId="21" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{1BDBFC0F-1DB0-4CE0-9283-C7753C9A1C08}" name="Datas" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{8685801F-D8EB-40A0-9379-8D5EFEBBEF4F}" name="Status"/>
     <tableColumn id="5" xr3:uid="{53569E75-C79C-4005-8928-F7E9BF8703BA}" name="Data de pagamento"/>
   </tableColumns>
@@ -4755,12 +4762,12 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{63127DFE-4527-4E0E-9664-43A07CD67B3D}" name="Tabela1578" displayName="Tabela1578" ref="M22:Q27" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{63127DFE-4527-4E0E-9664-43A07CD67B3D}" name="Tabela1578" displayName="Tabela1578" ref="M22:Q27" totalsRowShown="0" headerRowDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="M22:Q27" xr:uid="{63127DFE-4527-4E0E-9664-43A07CD67B3D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{2AA44ACE-540F-4EC9-8DA8-ECD552BD3268}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{760650C6-389C-4295-8C34-B36033C89850}" name="Valores" dataDxfId="20" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{F4885821-E248-4EE5-832C-6F9416CEC083}" name="Datas" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{760650C6-389C-4295-8C34-B36033C89850}" name="Valores" dataDxfId="17" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{F4885821-E248-4EE5-832C-6F9416CEC083}" name="Datas" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{828A104D-CCFF-4F7D-ADB2-A8653A6DD578}" name="Status"/>
     <tableColumn id="5" xr3:uid="{51637FDB-4A88-4509-A2ED-991C62817702}" name="Data de pagamento"/>
   </tableColumns>
@@ -4769,12 +4776,12 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F943793C-28BA-4AE6-A96C-468908CEA210}" name="Tabela159" displayName="Tabela159" ref="A37:E45" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F943793C-28BA-4AE6-A96C-468908CEA210}" name="Tabela159" displayName="Tabela159" ref="A37:E45" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A37:E45" xr:uid="{F943793C-28BA-4AE6-A96C-468908CEA210}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EEE7463A-3152-4BBA-9E33-329B5A4C388E}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{029AC23A-3574-41C8-9890-D9882B337248}" name="Valores" dataDxfId="16" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{F7A99513-2482-4119-B940-59605A481BB1}" name="Datas" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{029AC23A-3574-41C8-9890-D9882B337248}" name="Valores" dataDxfId="13" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{F7A99513-2482-4119-B940-59605A481BB1}" name="Datas" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{93D3F225-081B-4277-806B-D6575EF807D9}" name="Status"/>
     <tableColumn id="5" xr3:uid="{811E6842-9B4C-404A-8C92-A9B3728D5C0F}" name="Data de pagamento"/>
   </tableColumns>
@@ -4783,12 +4790,12 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5B63BC24-CE17-46CD-B259-72B4A0BD96CE}" name="Tabela1591011" displayName="Tabela1591011" ref="M37:Q48" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5B63BC24-CE17-46CD-B259-72B4A0BD96CE}" name="Tabela1591011" displayName="Tabela1591011" ref="M37:Q48" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="M37:Q48" xr:uid="{5B63BC24-CE17-46CD-B259-72B4A0BD96CE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5F8A2D41-67FA-423D-A670-B11AA757B295}" name="Despesas"/>
-    <tableColumn id="2" xr3:uid="{9C055CF7-F2CF-424A-8F52-68E280084806}" name="Valores" dataDxfId="12" dataCellStyle="Moeda"/>
-    <tableColumn id="3" xr3:uid="{5BA3B122-F3B3-4E85-9CDE-1BBB7AA88AA4}" name="Datas" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{9C055CF7-F2CF-424A-8F52-68E280084806}" name="Valores" dataDxfId="9" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{5BA3B122-F3B3-4E85-9CDE-1BBB7AA88AA4}" name="Datas" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{789D9805-C807-4637-B1C3-FA0E0BA74FF8}" name="Status"/>
     <tableColumn id="5" xr3:uid="{6E9FB04B-69A3-4F89-9EC2-785DCFC35D74}" name="Data de pagamento"/>
   </tableColumns>
@@ -5095,8 +5102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA32E0D-EAB5-470F-A070-3B1D486EDB0C}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5104,12 +5111,12 @@
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -5120,13 +5127,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:17" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
@@ -5968,7 +5980,9 @@
         <v>650.9</v>
       </c>
       <c r="I43" s="9"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="K43" s="3"/>
       <c r="M43" s="5" t="s">
         <v>39</v>
@@ -6015,7 +6029,7 @@
         <v>529.32000000000005</v>
       </c>
       <c r="C45" s="9"/>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="3"/>
@@ -6082,7 +6096,7 @@
       <c r="D52" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -6094,7 +6108,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="C53" s="7">
-        <v>44765</v>
+        <v>44826</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
@@ -6107,7 +6121,7 @@
         <v>33.950000000000003</v>
       </c>
       <c r="C54" s="7">
-        <v>44765</v>
+        <v>44826</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
@@ -6119,7 +6133,9 @@
       <c r="B55" s="6">
         <v>10.039999999999999</v>
       </c>
-      <c r="C55" s="7"/>
+      <c r="C55" s="7">
+        <v>44826</v>
+      </c>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
@@ -6130,7 +6146,9 @@
       <c r="B56" s="6">
         <v>14.9</v>
       </c>
-      <c r="C56" s="7"/>
+      <c r="C56" s="7">
+        <v>44828</v>
+      </c>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
@@ -6141,7 +6159,9 @@
       <c r="B57" s="6">
         <v>59.59</v>
       </c>
-      <c r="C57" s="7"/>
+      <c r="C57" s="7">
+        <v>44830</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
     </row>
@@ -6152,7 +6172,9 @@
       <c r="B58" s="6">
         <v>280.82</v>
       </c>
-      <c r="C58" s="7"/>
+      <c r="C58" s="7">
+        <v>44831</v>
+      </c>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
@@ -6163,7 +6185,9 @@
       <c r="B59" s="6">
         <v>20.8</v>
       </c>
-      <c r="C59" s="7"/>
+      <c r="C59" s="7">
+        <v>44832</v>
+      </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
@@ -6174,7 +6198,9 @@
       <c r="B60" s="6">
         <v>23.49</v>
       </c>
-      <c r="C60" s="7"/>
+      <c r="C60" s="7">
+        <v>44833</v>
+      </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
     </row>
@@ -6186,7 +6212,9 @@
         <f>14.9</f>
         <v>14.9</v>
       </c>
-      <c r="C61" s="7"/>
+      <c r="C61" s="7">
+        <v>44834</v>
+      </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
     </row>
@@ -6199,7 +6227,9 @@
         <v>460.94</v>
       </c>
       <c r="C62" s="9"/>
-      <c r="D62" s="3"/>
+      <c r="D62" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E62" s="3"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -6319,18 +6349,30 @@
       <c r="B81" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A4:A5"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="G38:H42">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Atraso">
+    <cfRule type="containsText" dxfId="44" priority="8" operator="containsText" text="Atraso">
       <formula>NOT(ISERROR(SEARCH("Atraso",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B62">
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="Em Aberto">
+      <formula>NOT(ISERROR(SEARCH("Em Aberto",B62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="containsText" dxfId="42" priority="2" operator="containsText" text="Em Aberto">
+      <formula>NOT(ISERROR(SEARCH("Em Aberto",D62)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="containsText" dxfId="41" priority="1" operator="containsText" text="Em Aberto">
+      <formula>NOT(ISERROR(SEARCH("Em Aberto",D45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D45" xr:uid="{52641133-0B5C-4B6E-83B5-FCBB05AA2F1C}">
-      <formula1>"Pago, Em Atraso"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J43 D62 D45" xr:uid="{1759CA56-6C82-454C-8B6B-2D707CDE0618}">
+      <formula1>"Pago, Em Aberto"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
criando o gráfico de arrecadação
</commit_message>
<xml_diff>
--- a/Planilha Cartão de Crédito/Cartão_de_Credito.xlsx
+++ b/Planilha Cartão de Crédito/Cartão_de_Credito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Gamer\Documents\Desenvolvimento 2022\Excel Estudos\Planilha Cartão de Crédito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510B79B4-F95D-46CD-980C-9D8BB854AF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33018BBB-8640-4DBF-A960-4AA1BA72C387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A65D1B47-B366-4730-B1BA-7EC03AAC71B1}"/>
   </bookViews>
@@ -5121,8 +5121,8 @@
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
     <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>